<commit_message>
evaluation results for uc1
</commit_message>
<xml_diff>
--- a/evaluation.xlsx
+++ b/evaluation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Lehner\Desktop\Repos\Papers\ECMFA_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B4D9D6-13E4-443D-B46F-646FA97BFF4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA3F4CE-CC6B-4746-82E5-19067A4F21C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-1330" windowWidth="19420" windowHeight="10420" xr2:uid="{726B67EE-5DA3-4D6A-83AC-2D94C3287F0D}"/>
+    <workbookView xWindow="11085" yWindow="795" windowWidth="12285" windowHeight="6705" xr2:uid="{726B67EE-5DA3-4D6A-83AC-2D94C3287F0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,17 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
-  <si>
-    <t>DT-enhanced UML</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>UML</t>
   </si>
   <si>
-    <t>Diff (%)</t>
-  </si>
-  <si>
     <t>DTDL</t>
   </si>
   <si>
@@ -77,17 +71,83 @@
     <t>UML4Vortolang</t>
   </si>
   <si>
-    <t>Not representable in DTDL</t>
+    <t>Create Classes</t>
+  </si>
+  <si>
+    <t>Create Properties</t>
+  </si>
+  <si>
+    <t>Create Associations</t>
+  </si>
+  <si>
+    <t>Create Operations</t>
+  </si>
+  <si>
+    <t>UC1 + config</t>
+  </si>
+  <si>
+    <t>UC1</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>DTUML</t>
+  </si>
+  <si>
+    <t>Delete Property Return Type</t>
+  </si>
+  <si>
+    <t>Change Class name</t>
+  </si>
+  <si>
+    <t>Change Property name</t>
+  </si>
+  <si>
+    <t>Change association multiplicity</t>
+  </si>
+  <si>
+    <t>Change Operation Parameter</t>
+  </si>
+  <si>
+    <t>Diff to DTUML</t>
+  </si>
+  <si>
+    <t>Diff to UML</t>
+  </si>
+  <si>
+    <t>Step</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -110,13 +170,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -429,80 +498,456 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CF141AC-6C1A-4378-B63E-21F7B9A42F11}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>13</v>
+      <c r="G1" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D2">
-        <v>5</v>
-      </c>
-      <c r="E2">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1">
         <f>(D2-C2)/C2</f>
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="G2" s="1">
+        <f>(F2-D2)/D2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>22</v>
+      </c>
+      <c r="D3">
+        <v>27</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:E6" si="0">(D3-C3)/C3</f>
+        <v>0.22727272727272727</v>
+      </c>
+      <c r="F3">
+        <v>22</v>
+      </c>
+      <c r="G3" s="1">
+        <f>(F3-D3)/D3</f>
+        <v>-0.18518518518518517</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>70</v>
+      </c>
+      <c r="D4">
+        <v>70</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>23</v>
+      </c>
+      <c r="G4" s="1">
+        <f>(F4-D4)/D4</f>
+        <v>-0.67142857142857137</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>16</v>
+      </c>
+      <c r="D5">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1">
+        <f>(F5-D5)/D5</f>
+        <v>-0.375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2">
+        <f>SUM(C2:C5)</f>
+        <v>124</v>
+      </c>
+      <c r="D6" s="2">
+        <f>SUM(D2:D5)</f>
+        <v>129</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>4.0322580645161289E-2</v>
+      </c>
+      <c r="F6" s="2">
+        <f>SUM(F2:F5)</f>
+        <v>71</v>
+      </c>
+      <c r="G6" s="3">
+        <f>(F6-D6)/D6</f>
+        <v>-0.44961240310077522</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" ref="E7:E12" si="1">(D7-C7)/C7</f>
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <f>(F7-D7)/D7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1">
+        <f>(F8-D8)/D8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1">
+        <f>(F9-D9)/D9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10" s="1">
+        <f>(F10-D10)/D10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11" s="1">
+        <f>(F11-D11)/D11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <f>SUM(C7:C11)</f>
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ref="D12:F12" si="2">SUM(D7:D11)</f>
+        <v>14</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="1"/>
+        <v>1.8</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="G12" s="1">
+        <f>(F12-D12)/D12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17">
+        <v>32</v>
+      </c>
+      <c r="E17" s="1">
+        <f>(D17-C17)/C17</f>
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>32</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" ref="G17:G21" si="3">(F17-D17)/D17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18">
+        <v>22</v>
+      </c>
+      <c r="D18">
+        <v>41</v>
+      </c>
+      <c r="E18" s="1">
+        <f>(D18-C18)/C18</f>
+        <v>0.86363636363636365</v>
+      </c>
+      <c r="F18">
+        <v>36</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="3"/>
+        <v>-0.12195121951219512</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19">
+        <v>70</v>
+      </c>
+      <c r="D19">
+        <v>88</v>
+      </c>
+      <c r="E19" s="1">
+        <f>(D19-C19)/C19</f>
+        <v>0.25714285714285712</v>
+      </c>
+      <c r="F19">
+        <v>37</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="3"/>
+        <v>-0.57954545454545459</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20">
+        <v>16</v>
+      </c>
+      <c r="D20">
+        <v>20</v>
+      </c>
+      <c r="E20" s="1">
+        <f>(D20-C20)/C20</f>
+        <v>0.25</v>
+      </c>
+      <c r="F20">
+        <v>14</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="3"/>
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="2">
+        <f>SUM(C17:C20)</f>
+        <v>124</v>
+      </c>
+      <c r="D21" s="2">
+        <f t="shared" ref="D21:F21" si="4">SUM(D17:D20)</f>
+        <v>181</v>
+      </c>
+      <c r="E21" s="3">
+        <f>(D21-C21)/C21</f>
+        <v>0.45967741935483869</v>
+      </c>
+      <c r="F21" s="2">
+        <f t="shared" si="4"/>
+        <v>119</v>
+      </c>
+      <c r="G21" s="3">
+        <f t="shared" si="3"/>
+        <v>-0.34254143646408841</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A21:B21"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -521,41 +966,41 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add use case 2 models + evaluation data
</commit_message>
<xml_diff>
--- a/evaluation.xlsx
+++ b/evaluation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Lehner\Desktop\Repos\Papers\ECMFA_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA3F4CE-CC6B-4746-82E5-19067A4F21C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D12EE94-1B40-4749-96A4-86ADC9F422E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11085" yWindow="795" windowWidth="12285" windowHeight="6705" xr2:uid="{726B67EE-5DA3-4D6A-83AC-2D94C3287F0D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="17520" windowHeight="12600" xr2:uid="{726B67EE-5DA3-4D6A-83AC-2D94C3287F0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
   <si>
     <t>UML</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Step</t>
+  </si>
+  <si>
+    <t>UC2</t>
   </si>
 </sst>
 </file>
@@ -179,10 +182,10 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -498,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CF141AC-6C1A-4378-B63E-21F7B9A42F11}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,7 +558,7 @@
         <v>16</v>
       </c>
       <c r="G2" s="1">
-        <f>(F2-D2)/D2</f>
+        <f t="shared" ref="G2:G20" si="0">(F2-D2)/D2</f>
         <v>0</v>
       </c>
     </row>
@@ -573,14 +576,14 @@
         <v>27</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E6" si="0">(D3-C3)/C3</f>
+        <f t="shared" ref="E3:E6" si="1">(D3-C3)/C3</f>
         <v>0.22727272727272727</v>
       </c>
       <c r="F3">
         <v>22</v>
       </c>
       <c r="G3" s="1">
-        <f>(F3-D3)/D3</f>
+        <f t="shared" si="0"/>
         <v>-0.18518518518518517</v>
       </c>
     </row>
@@ -598,14 +601,14 @@
         <v>70</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F4">
         <v>23</v>
       </c>
       <c r="G4" s="1">
-        <f>(F4-D4)/D4</f>
+        <f t="shared" si="0"/>
         <v>-0.67142857142857137</v>
       </c>
     </row>
@@ -623,22 +626,22 @@
         <v>16</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F5">
         <v>10</v>
       </c>
       <c r="G5" s="1">
-        <f>(F5-D5)/D5</f>
+        <f t="shared" si="0"/>
         <v>-0.375</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="2">
@@ -650,7 +653,7 @@
         <v>129</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.0322580645161289E-2</v>
       </c>
       <c r="F6" s="2">
@@ -658,7 +661,7 @@
         <v>71</v>
       </c>
       <c r="G6" s="3">
-        <f>(F6-D6)/D6</f>
+        <f t="shared" si="0"/>
         <v>-0.44961240310077522</v>
       </c>
     </row>
@@ -676,14 +679,14 @@
         <v>2</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" ref="E7:E12" si="1">(D7-C7)/C7</f>
+        <f t="shared" ref="E7:E18" si="2">(D7-C7)/C7</f>
         <v>1</v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
       <c r="G7" s="1">
-        <f>(F7-D7)/D7</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -701,14 +704,14 @@
         <v>3</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="F8">
         <v>3</v>
       </c>
       <c r="G8" s="1">
-        <f>(F8-D8)/D8</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -726,14 +729,14 @@
         <v>3</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="F9">
         <v>3</v>
       </c>
       <c r="G9" s="1">
-        <f>(F9-D9)/D9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -751,14 +754,14 @@
         <v>3</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="F10">
         <v>3</v>
       </c>
       <c r="G10" s="1">
-        <f>(F10-D10)/D10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -776,22 +779,22 @@
         <v>3</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="F11">
         <v>3</v>
       </c>
       <c r="G11" s="1">
-        <f>(F11-D11)/D11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C12">
@@ -799,151 +802,305 @@
         <v>5</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="D12:F12" si="2">SUM(D7:D11)</f>
+        <f t="shared" ref="D12:F12" si="3">SUM(D7:D11)</f>
         <v>14</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.8</v>
       </c>
       <c r="F12">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13" s="1">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>6</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>30</v>
+      </c>
+      <c r="D14">
+        <v>34</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="2"/>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="F14">
+        <v>30</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.11764705882352941</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>24</v>
+      </c>
+      <c r="D15">
+        <v>24</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>9</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.625</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="1">
-        <f>(F12-D12)/D12</f>
-        <v>0</v>
+      <c r="C16">
+        <v>34</v>
+      </c>
+      <c r="D16">
+        <v>34</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>28</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.17647058823529413</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17">
+        <f>SUM(C13:C16)</f>
+        <v>94</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ref="D17:G17" si="4">SUM(D13:D16)</f>
+        <v>98</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="2"/>
+        <v>4.2553191489361701E-2</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="4"/>
+        <v>73</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.25510204081632654</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="E18" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G18" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="G19" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="G20" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B27" t="s">
         <v>11</v>
       </c>
-      <c r="C17">
-        <v>16</v>
-      </c>
-      <c r="D17">
+      <c r="C27">
+        <v>16</v>
+      </c>
+      <c r="D27">
         <v>32</v>
       </c>
-      <c r="E17" s="1">
-        <f>(D17-C17)/C17</f>
+      <c r="E27" s="1">
+        <f>(D27-C27)/C27</f>
         <v>1</v>
       </c>
-      <c r="F17">
+      <c r="F27">
         <v>32</v>
       </c>
-      <c r="G17" s="1">
-        <f t="shared" ref="G17:G21" si="3">(F17-D17)/D17</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="G27" s="1">
+        <f t="shared" ref="G27:G31" si="5">(F27-D27)/D27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>15</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B28" t="s">
         <v>12</v>
       </c>
-      <c r="C18">
+      <c r="C28">
         <v>22</v>
       </c>
-      <c r="D18">
+      <c r="D28">
         <v>41</v>
       </c>
-      <c r="E18" s="1">
-        <f>(D18-C18)/C18</f>
+      <c r="E28" s="1">
+        <f>(D28-C28)/C28</f>
         <v>0.86363636363636365</v>
       </c>
-      <c r="F18">
+      <c r="F28">
         <v>36</v>
       </c>
-      <c r="G18" s="1">
-        <f t="shared" si="3"/>
+      <c r="G28" s="1">
+        <f t="shared" si="5"/>
         <v>-0.12195121951219512</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>15</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B29" t="s">
         <v>13</v>
       </c>
-      <c r="C19">
+      <c r="C29">
         <v>70</v>
       </c>
-      <c r="D19">
+      <c r="D29">
         <v>88</v>
       </c>
-      <c r="E19" s="1">
-        <f>(D19-C19)/C19</f>
+      <c r="E29" s="1">
+        <f>(D29-C29)/C29</f>
         <v>0.25714285714285712</v>
       </c>
-      <c r="F19">
+      <c r="F29">
         <v>37</v>
       </c>
-      <c r="G19" s="1">
-        <f t="shared" si="3"/>
+      <c r="G29" s="1">
+        <f t="shared" si="5"/>
         <v>-0.57954545454545459</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>15</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B30" t="s">
         <v>14</v>
       </c>
-      <c r="C20">
-        <v>16</v>
-      </c>
-      <c r="D20">
+      <c r="C30">
+        <v>16</v>
+      </c>
+      <c r="D30">
         <v>20</v>
       </c>
-      <c r="E20" s="1">
-        <f>(D20-C20)/C20</f>
+      <c r="E30" s="1">
+        <f>(D30-C30)/C30</f>
         <v>0.25</v>
       </c>
-      <c r="F20">
+      <c r="F30">
         <v>14</v>
       </c>
-      <c r="G20" s="1">
-        <f t="shared" si="3"/>
+      <c r="G30" s="1">
+        <f t="shared" si="5"/>
         <v>-0.3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="2">
-        <f>SUM(C17:C20)</f>
+      <c r="B31" s="5"/>
+      <c r="C31" s="2">
+        <f>SUM(C27:C30)</f>
         <v>124</v>
       </c>
-      <c r="D21" s="2">
-        <f t="shared" ref="D21:F21" si="4">SUM(D17:D20)</f>
+      <c r="D31" s="2">
+        <f t="shared" ref="D31:F31" si="6">SUM(D27:D30)</f>
         <v>181</v>
       </c>
-      <c r="E21" s="3">
-        <f>(D21-C21)/C21</f>
+      <c r="E31" s="3">
+        <f>(D31-C31)/C31</f>
         <v>0.45967741935483869</v>
       </c>
-      <c r="F21" s="2">
-        <f t="shared" si="4"/>
+      <c r="F31" s="2">
+        <f t="shared" si="6"/>
         <v>119</v>
       </c>
-      <c r="G21" s="3">
-        <f t="shared" si="3"/>
+      <c r="G31" s="3">
+        <f t="shared" si="5"/>
         <v>-0.34254143646408841</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A31:B31"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>